<commit_message>
change to pre-week data
</commit_message>
<xml_diff>
--- a/data/samplesize.xlsx
+++ b/data/samplesize.xlsx
@@ -432,16 +432,16 @@
         <v>7</v>
       </c>
       <c r="G2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H2">
         <v>34</v>
       </c>
       <c r="I2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J2">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3">
@@ -451,31 +451,31 @@
         </is>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3">
         <v>10</v>
       </c>
       <c r="F3">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G3">
         <v>10</v>
       </c>
       <c r="H3">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I3">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J3">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4">
@@ -485,31 +485,31 @@
         </is>
       </c>
       <c r="B4">
-        <v>906</v>
+        <v>864</v>
       </c>
       <c r="C4">
-        <v>1091</v>
+        <v>1069</v>
       </c>
       <c r="D4">
-        <v>888</v>
+        <v>845</v>
       </c>
       <c r="E4">
-        <v>882</v>
+        <v>839</v>
       </c>
       <c r="F4">
-        <v>1046</v>
+        <v>1026</v>
       </c>
       <c r="G4">
-        <v>886</v>
+        <v>857</v>
       </c>
       <c r="H4">
-        <v>2885</v>
+        <v>2778</v>
       </c>
       <c r="I4">
-        <v>2814</v>
+        <v>2722</v>
       </c>
       <c r="J4">
-        <v>5699</v>
+        <v>5500</v>
       </c>
     </row>
     <row r="5">
@@ -553,31 +553,31 @@
         </is>
       </c>
       <c r="B6">
-        <v>684</v>
+        <v>727</v>
       </c>
       <c r="C6">
-        <v>489</v>
+        <v>512</v>
       </c>
       <c r="D6">
-        <v>595</v>
+        <v>639</v>
       </c>
       <c r="E6">
-        <v>492</v>
+        <v>535</v>
       </c>
       <c r="F6">
-        <v>694</v>
+        <v>717</v>
       </c>
       <c r="G6">
-        <v>477</v>
+        <v>505</v>
       </c>
       <c r="H6">
-        <v>1768</v>
+        <v>1878</v>
       </c>
       <c r="I6">
-        <v>1663</v>
+        <v>1757</v>
       </c>
       <c r="J6">
-        <v>3431</v>
+        <v>3635</v>
       </c>
     </row>
     <row r="7">
@@ -621,7 +621,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -695,13 +695,13 @@
         <v>13</v>
       </c>
       <c r="E2">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2">
         <v>7</v>
       </c>
       <c r="G2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H2">
         <v>34</v>
@@ -716,544 +716,578 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Epithelium</t>
+          <t>EN_Lymph</t>
         </is>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="J3">
-        <v>69</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>GC_Active CL</t>
+          <t>Epithelium</t>
         </is>
       </c>
       <c r="B4">
-        <v>148</v>
+        <v>9</v>
       </c>
       <c r="C4">
-        <v>103</v>
+        <v>10</v>
       </c>
       <c r="D4">
-        <v>121</v>
+        <v>14</v>
       </c>
       <c r="E4">
-        <v>110</v>
+        <v>10</v>
       </c>
       <c r="F4">
-        <v>99</v>
+        <v>11</v>
       </c>
       <c r="G4">
-        <v>97</v>
+        <v>10</v>
       </c>
       <c r="H4">
-        <v>372</v>
+        <v>33</v>
       </c>
       <c r="I4">
-        <v>306</v>
+        <v>31</v>
       </c>
       <c r="J4">
-        <v>678</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>GC_Antral</t>
+          <t>GC_Active CL</t>
         </is>
       </c>
       <c r="B5">
-        <v>437</v>
+        <v>9</v>
       </c>
       <c r="C5">
-        <v>671</v>
+        <v>3</v>
       </c>
       <c r="D5">
-        <v>512</v>
+        <v>8</v>
       </c>
       <c r="E5">
-        <v>454</v>
+        <v>2</v>
       </c>
       <c r="F5">
-        <v>596</v>
+        <v>3</v>
       </c>
       <c r="G5">
-        <v>541</v>
+        <v>9</v>
       </c>
       <c r="H5">
-        <v>1620</v>
+        <v>20</v>
       </c>
       <c r="I5">
-        <v>1591</v>
+        <v>14</v>
       </c>
       <c r="J5">
-        <v>3211</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>GC_Luteinizing</t>
+          <t>GC_Antral</t>
         </is>
       </c>
       <c r="B6">
-        <v>145</v>
+        <v>459</v>
       </c>
       <c r="C6">
-        <v>75</v>
+        <v>680</v>
       </c>
       <c r="D6">
-        <v>70</v>
+        <v>532</v>
       </c>
       <c r="E6">
-        <v>111</v>
+        <v>450</v>
       </c>
       <c r="F6">
-        <v>57</v>
+        <v>590</v>
       </c>
       <c r="G6">
-        <v>57</v>
+        <v>528</v>
       </c>
       <c r="H6">
-        <v>290</v>
+        <v>1671</v>
       </c>
       <c r="I6">
-        <v>225</v>
+        <v>1568</v>
       </c>
       <c r="J6">
-        <v>515</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>GC_Mitotic</t>
+          <t>GC_Atretic</t>
         </is>
       </c>
       <c r="B7">
-        <v>109</v>
+        <v>27</v>
       </c>
       <c r="C7">
-        <v>198</v>
+        <v>18</v>
       </c>
       <c r="D7">
-        <v>118</v>
+        <v>15</v>
       </c>
       <c r="E7">
-        <v>161</v>
+        <v>20</v>
       </c>
       <c r="F7">
-        <v>239</v>
+        <v>20</v>
       </c>
       <c r="G7">
-        <v>161</v>
+        <v>21</v>
       </c>
       <c r="H7">
-        <v>425</v>
+        <v>60</v>
       </c>
       <c r="I7">
-        <v>561</v>
+        <v>61</v>
       </c>
       <c r="J7">
-        <v>986</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>GC_Mural</t>
+          <t>GC_Luteinizing</t>
         </is>
       </c>
       <c r="B8">
-        <v>11</v>
+        <v>186</v>
       </c>
       <c r="C8">
-        <v>6</v>
+        <v>110</v>
       </c>
       <c r="D8">
-        <v>10</v>
+        <v>102</v>
       </c>
       <c r="E8">
-        <v>6</v>
+        <v>150</v>
       </c>
       <c r="F8">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="G8">
-        <v>4</v>
+        <v>74</v>
       </c>
       <c r="H8">
-        <v>27</v>
+        <v>398</v>
       </c>
       <c r="I8">
-        <v>17</v>
+        <v>308</v>
       </c>
       <c r="J8">
-        <v>44</v>
+        <v>706</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>GC_Preantral</t>
+          <t>GC_Mitotic</t>
         </is>
       </c>
       <c r="B9">
-        <v>28</v>
+        <v>112</v>
       </c>
       <c r="C9">
-        <v>14</v>
+        <v>208</v>
       </c>
       <c r="D9">
-        <v>35</v>
+        <v>124</v>
       </c>
       <c r="E9">
-        <v>22</v>
+        <v>168</v>
       </c>
       <c r="F9">
-        <v>32</v>
+        <v>259</v>
       </c>
       <c r="G9">
-        <v>24</v>
+        <v>181</v>
       </c>
       <c r="H9">
-        <v>77</v>
+        <v>444</v>
       </c>
       <c r="I9">
-        <v>78</v>
+        <v>608</v>
       </c>
       <c r="J9">
-        <v>155</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>GC_Regressing CL</t>
+          <t>GC_Preantral</t>
         </is>
       </c>
       <c r="B10">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="C10">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D10">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="E10">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="F10">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="G10">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="H10">
-        <v>72</v>
+        <v>132</v>
       </c>
       <c r="I10">
-        <v>33</v>
+        <v>142</v>
       </c>
       <c r="J10">
-        <v>105</v>
+        <v>274</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>I_Macrophage</t>
+          <t>GC_Regressing CL</t>
         </is>
       </c>
       <c r="B11">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C11">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E11">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F11">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G11">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="H11">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="I11">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="J11">
-        <v>76</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>M_Early Theca</t>
+          <t>I_Macrophage</t>
         </is>
       </c>
       <c r="B12">
-        <v>87</v>
+        <v>15</v>
       </c>
       <c r="C12">
-        <v>95</v>
+        <v>13</v>
       </c>
       <c r="D12">
-        <v>94</v>
+        <v>10</v>
       </c>
       <c r="E12">
-        <v>79</v>
+        <v>12</v>
       </c>
       <c r="F12">
-        <v>140</v>
+        <v>10</v>
       </c>
       <c r="G12">
-        <v>69</v>
+        <v>16</v>
       </c>
       <c r="H12">
-        <v>276</v>
+        <v>38</v>
       </c>
       <c r="I12">
-        <v>288</v>
+        <v>38</v>
       </c>
       <c r="J12">
-        <v>564</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>M_Fibroblast-like Stroma</t>
+          <t>M_Early Theca</t>
         </is>
       </c>
       <c r="B13">
-        <v>92</v>
+        <v>113</v>
       </c>
       <c r="C13">
-        <v>68</v>
+        <v>126</v>
       </c>
       <c r="D13">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="E13">
-        <v>55</v>
+        <v>102</v>
       </c>
       <c r="F13">
-        <v>90</v>
+        <v>179</v>
       </c>
       <c r="G13">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="H13">
-        <v>261</v>
+        <v>350</v>
       </c>
       <c r="I13">
-        <v>212</v>
+        <v>370</v>
       </c>
       <c r="J13">
-        <v>473</v>
+        <v>720</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>M_Pericyte</t>
+          <t>M_Fibroblast-like Stroma</t>
         </is>
       </c>
       <c r="B14">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C14">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="D14">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="E14">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F14">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G14">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="H14">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="I14">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="J14">
-        <v>148</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>M_Smooth Muscle</t>
+          <t>M_Pericyte</t>
         </is>
       </c>
       <c r="B15">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C15">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D15">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="E15">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F15">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="G15">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H15">
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="I15">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="J15">
-        <v>140</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>M_Steroidogenic Stroma</t>
+          <t>M_Smooth Muscle</t>
         </is>
       </c>
       <c r="B16">
-        <v>341</v>
+        <v>12</v>
       </c>
       <c r="C16">
-        <v>200</v>
+        <v>5</v>
       </c>
       <c r="D16">
-        <v>238</v>
+        <v>9</v>
       </c>
       <c r="E16">
-        <v>218</v>
+        <v>11</v>
       </c>
       <c r="F16">
-        <v>303</v>
+        <v>13</v>
       </c>
       <c r="G16">
-        <v>184</v>
+        <v>11</v>
       </c>
       <c r="H16">
-        <v>779</v>
+        <v>26</v>
       </c>
       <c r="I16">
-        <v>705</v>
+        <v>35</v>
       </c>
       <c r="J16">
-        <v>1484</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>M_Steroidogenic Theca</t>
+          <t>M_Steroidogenic Stroma</t>
         </is>
       </c>
       <c r="B17">
-        <v>114</v>
+        <v>419</v>
       </c>
       <c r="C17">
-        <v>86</v>
+        <v>249</v>
       </c>
       <c r="D17">
-        <v>97</v>
+        <v>325</v>
       </c>
       <c r="E17">
-        <v>106</v>
+        <v>276</v>
       </c>
       <c r="F17">
-        <v>114</v>
+        <v>359</v>
       </c>
       <c r="G17">
-        <v>110</v>
+        <v>226</v>
       </c>
       <c r="H17">
-        <v>297</v>
+        <v>993</v>
       </c>
       <c r="I17">
-        <v>330</v>
+        <v>861</v>
       </c>
       <c r="J17">
-        <v>627</v>
+        <v>1854</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>M_Steroidogenic Theca</t>
+        </is>
+      </c>
+      <c r="B18">
+        <v>150</v>
+      </c>
+      <c r="C18">
+        <v>99</v>
+      </c>
+      <c r="D18">
+        <v>135</v>
+      </c>
+      <c r="E18">
+        <v>126</v>
+      </c>
+      <c r="F18">
+        <v>129</v>
+      </c>
+      <c r="G18">
+        <v>144</v>
+      </c>
+      <c r="H18">
+        <v>384</v>
+      </c>
+      <c r="I18">
+        <v>399</v>
+      </c>
+      <c r="J18">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="B18">
+      <c r="B19">
         <v>1628</v>
       </c>
-      <c r="C18">
+      <c r="C19">
         <v>1611</v>
       </c>
-      <c r="D18">
+      <c r="D19">
         <v>1521</v>
       </c>
-      <c r="E18">
+      <c r="E19">
         <v>1410</v>
       </c>
-      <c r="F18">
+      <c r="F19">
         <v>1771</v>
       </c>
-      <c r="G18">
+      <c r="G19">
         <v>1416</v>
       </c>
-      <c r="H18">
+      <c r="H19">
         <v>4760</v>
       </c>
-      <c r="I18">
+      <c r="I19">
         <v>4597</v>
       </c>
-      <c r="J18">
+      <c r="J19">
         <v>9357</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Mostly finalized for publication
needs a couple last changes
</commit_message>
<xml_diff>
--- a/data/samplesize.xlsx
+++ b/data/samplesize.xlsx
@@ -8,7 +8,9 @@
   </bookViews>
   <sheets>
     <sheet name="Level0" sheetId="1" r:id="rId1"/>
-    <sheet name="Level1" sheetId="2" r:id="rId2"/>
+    <sheet name="Level0-prop" sheetId="2" r:id="rId2"/>
+    <sheet name="Level1" sheetId="3" r:id="rId3"/>
+    <sheet name="Level1-prop" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -485,31 +487,31 @@
         </is>
       </c>
       <c r="B4">
-        <v>993</v>
+        <v>990</v>
       </c>
       <c r="C4">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="D4">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="E4">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="F4">
-        <v>1079</v>
+        <v>1075</v>
       </c>
       <c r="G4">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="H4">
-        <v>3059</v>
+        <v>3055</v>
       </c>
       <c r="I4">
-        <v>3041</v>
+        <v>3036</v>
       </c>
       <c r="J4">
-        <v>6100</v>
+        <v>6091</v>
       </c>
     </row>
     <row r="5">
@@ -553,31 +555,31 @@
         </is>
       </c>
       <c r="B6">
-        <v>767</v>
+        <v>770</v>
       </c>
       <c r="C6">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="D6">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="E6">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="F6">
-        <v>780</v>
+        <v>784</v>
       </c>
       <c r="G6">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="H6">
-        <v>1989</v>
+        <v>1993</v>
       </c>
       <c r="I6">
-        <v>1941</v>
+        <v>1946</v>
       </c>
       <c r="J6">
-        <v>3930</v>
+        <v>3939</v>
       </c>
     </row>
     <row r="7">
@@ -620,6 +622,275 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Cell Type</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>2262</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>2263</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>2264</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>2265</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>2266</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>2267</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>CTRL</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Endothelium</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>0.008282716731087797</v>
+      </c>
+      <c r="C2">
+        <v>0.007479861910241657</v>
+      </c>
+      <c r="D2">
+        <v>0.01518833535844471</v>
+      </c>
+      <c r="E2">
+        <v>0.01075268817204301</v>
+      </c>
+      <c r="F2">
+        <v>0.005780346820809248</v>
+      </c>
+      <c r="G2">
+        <v>0.02493606138107417</v>
+      </c>
+      <c r="H2">
+        <v>0.01020211742059673</v>
+      </c>
+      <c r="I2">
+        <v>0.0132269986383972</v>
+      </c>
+      <c r="J2">
+        <v>0.01170665634674923</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Epithelium</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>0.00717835450027609</v>
+      </c>
+      <c r="C3">
+        <v>0.00805523590333717</v>
+      </c>
+      <c r="D3">
+        <v>0.01093560145808019</v>
+      </c>
+      <c r="E3">
+        <v>0.005973715651135006</v>
+      </c>
+      <c r="F3">
+        <v>0.01050972149238045</v>
+      </c>
+      <c r="G3">
+        <v>0.008951406649616368</v>
+      </c>
+      <c r="H3">
+        <v>0.008662175168431183</v>
+      </c>
+      <c r="I3">
+        <v>0.008558646177786422</v>
+      </c>
+      <c r="J3">
+        <v>0.008610681114551084</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Granulosa</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>0.5466593042517945</v>
+      </c>
+      <c r="C4">
+        <v>0.6599539700805523</v>
+      </c>
+      <c r="D4">
+        <v>0.5577156743620899</v>
+      </c>
+      <c r="E4">
+        <v>0.6075268817204301</v>
+      </c>
+      <c r="F4">
+        <v>0.5648975302154493</v>
+      </c>
+      <c r="G4">
+        <v>0.6035805626598465</v>
+      </c>
+      <c r="H4">
+        <v>0.588065447545717</v>
+      </c>
+      <c r="I4">
+        <v>0.5905465862672632</v>
+      </c>
+      <c r="J4">
+        <v>0.5892995356037152</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Immune</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>0.01270016565433462</v>
+      </c>
+      <c r="C5">
+        <v>0.00805523590333717</v>
+      </c>
+      <c r="D5">
+        <v>0.007290400972053463</v>
+      </c>
+      <c r="E5">
+        <v>0.01015531660692951</v>
+      </c>
+      <c r="F5">
+        <v>0.006831318970047294</v>
+      </c>
+      <c r="G5">
+        <v>0.0108695652173913</v>
+      </c>
+      <c r="H5">
+        <v>0.009432146294513956</v>
+      </c>
+      <c r="I5">
+        <v>0.009142190235362771</v>
+      </c>
+      <c r="J5">
+        <v>0.009287925696594427</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Mesenchyme</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>0.4251794588625069</v>
+      </c>
+      <c r="C6">
+        <v>0.3164556962025317</v>
+      </c>
+      <c r="D6">
+        <v>0.4088699878493317</v>
+      </c>
+      <c r="E6">
+        <v>0.3655913978494624</v>
+      </c>
+      <c r="F6">
+        <v>0.4119810825013137</v>
+      </c>
+      <c r="G6">
+        <v>0.3516624040920716</v>
+      </c>
+      <c r="H6">
+        <v>0.3836381135707411</v>
+      </c>
+      <c r="I6">
+        <v>0.3785255786811904</v>
+      </c>
+      <c r="J6">
+        <v>0.3810952012383901</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J18"/>
   <sheetViews>
@@ -754,31 +1025,31 @@
         </is>
       </c>
       <c r="B4">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C4">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E4">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F4">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G4">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H4">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="I4">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="J4">
-        <v>239</v>
+        <v>221</v>
       </c>
     </row>
     <row r="5">
@@ -788,7 +1059,7 @@
         </is>
       </c>
       <c r="B5">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5">
         <v>25</v>
@@ -797,7 +1068,7 @@
         <v>46</v>
       </c>
       <c r="E5">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F5">
         <v>56</v>
@@ -806,13 +1077,13 @@
         <v>36</v>
       </c>
       <c r="H5">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I5">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="J5">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="6">
@@ -825,28 +1096,28 @@
         <v>353</v>
       </c>
       <c r="C6">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D6">
         <v>207</v>
       </c>
       <c r="E6">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="F6">
         <v>146</v>
       </c>
       <c r="G6">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="H6">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="I6">
         <v>598</v>
       </c>
       <c r="J6">
-        <v>1380</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="7">
@@ -856,31 +1127,31 @@
         </is>
       </c>
       <c r="B7">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C7">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D7">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E7">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F7">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="G7">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H7">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="I7">
-        <v>728</v>
+        <v>721</v>
       </c>
       <c r="J7">
-        <v>1220</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="8">
@@ -890,31 +1161,31 @@
         </is>
       </c>
       <c r="B8">
-        <v>402</v>
+        <v>411</v>
       </c>
       <c r="C8">
-        <v>634</v>
+        <v>637</v>
       </c>
       <c r="D8">
-        <v>483</v>
+        <v>487</v>
       </c>
       <c r="E8">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F8">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="G8">
-        <v>502</v>
+        <v>507</v>
       </c>
       <c r="H8">
-        <v>1519</v>
+        <v>1535</v>
       </c>
       <c r="I8">
-        <v>1482</v>
+        <v>1488</v>
       </c>
       <c r="J8">
-        <v>3001</v>
+        <v>3023</v>
       </c>
     </row>
     <row r="9">
@@ -992,16 +1263,16 @@
         </is>
       </c>
       <c r="B11">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C11">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D11">
         <v>102</v>
       </c>
       <c r="E11">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F11">
         <v>205</v>
@@ -1010,13 +1281,13 @@
         <v>100</v>
       </c>
       <c r="H11">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="I11">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="J11">
-        <v>744</v>
+        <v>747</v>
       </c>
     </row>
     <row r="12">
@@ -1026,7 +1297,7 @@
         </is>
       </c>
       <c r="B12">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C12">
         <v>9</v>
@@ -1044,13 +1315,13 @@
         <v>6</v>
       </c>
       <c r="H12">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I12">
         <v>28</v>
       </c>
       <c r="J12">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13">
@@ -1128,31 +1399,31 @@
         </is>
       </c>
       <c r="B15">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C15">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D15">
         <v>299</v>
       </c>
       <c r="E15">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F15">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G15">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H15">
-        <v>894</v>
+        <v>891</v>
       </c>
       <c r="I15">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="J15">
-        <v>1658</v>
+        <v>1651</v>
       </c>
     </row>
     <row r="16">
@@ -1162,31 +1433,31 @@
         </is>
       </c>
       <c r="B16">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C16">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D16">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E16">
         <v>228</v>
       </c>
       <c r="F16">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="G16">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="H16">
-        <v>567</v>
+        <v>571</v>
       </c>
       <c r="I16">
-        <v>613</v>
+        <v>621</v>
       </c>
       <c r="J16">
-        <v>1180</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="17">
@@ -1255,6 +1526,649 @@
       </c>
       <c r="J18">
         <v>10336</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Cell Type</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>2262</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>2263</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>2264</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>2265</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>2266</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>2267</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>CTRL</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Endothelium</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>0.1209677419354839</v>
+      </c>
+      <c r="C2">
+        <v>0.05701754385964912</v>
+      </c>
+      <c r="D2">
+        <v>0.1851851851851852</v>
+      </c>
+      <c r="E2">
+        <v>0.08</v>
+      </c>
+      <c r="F2">
+        <v>0.03806228373702422</v>
+      </c>
+      <c r="G2">
+        <v>0.1884057971014493</v>
+      </c>
+      <c r="H2">
+        <v>0.108829568788501</v>
+      </c>
+      <c r="I2">
+        <v>0.09431345353675451</v>
+      </c>
+      <c r="J2">
+        <v>0.1001655629139073</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Epithelium</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>0.1048387096774194</v>
+      </c>
+      <c r="C3">
+        <v>0.06140350877192982</v>
+      </c>
+      <c r="D3">
+        <v>0.1333333333333333</v>
+      </c>
+      <c r="E3">
+        <v>0.04444444444444445</v>
+      </c>
+      <c r="F3">
+        <v>0.06920415224913495</v>
+      </c>
+      <c r="G3">
+        <v>0.06763285024154589</v>
+      </c>
+      <c r="H3">
+        <v>0.09240246406570841</v>
+      </c>
+      <c r="I3">
+        <v>0.06102635228848821</v>
+      </c>
+      <c r="J3">
+        <v>0.07367549668874172</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>GC_Atretic</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>0.4032258064516129</v>
+      </c>
+      <c r="C4">
+        <v>0.1666666666666667</v>
+      </c>
+      <c r="D4">
+        <v>0.3185185185185185</v>
+      </c>
+      <c r="E4">
+        <v>0.1022222222222222</v>
+      </c>
+      <c r="F4">
+        <v>0.1038062283737024</v>
+      </c>
+      <c r="G4">
+        <v>0.178743961352657</v>
+      </c>
+      <c r="H4">
+        <v>0.2689938398357289</v>
+      </c>
+      <c r="I4">
+        <v>0.1248266296809986</v>
+      </c>
+      <c r="J4">
+        <v>0.1829470198675497</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>GC_Cumulus</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>0.4193548387096774</v>
+      </c>
+      <c r="C5">
+        <v>0.1096491228070175</v>
+      </c>
+      <c r="D5">
+        <v>0.3407407407407407</v>
+      </c>
+      <c r="E5">
+        <v>0.2088888888888889</v>
+      </c>
+      <c r="F5">
+        <v>0.1937716262975779</v>
+      </c>
+      <c r="G5">
+        <v>0.1739130434782609</v>
+      </c>
+      <c r="H5">
+        <v>0.2525667351129364</v>
+      </c>
+      <c r="I5">
+        <v>0.1927877947295423</v>
+      </c>
+      <c r="J5">
+        <v>0.216887417218543</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>GC_Luteinizing and CL</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>2.846774193548387</v>
+      </c>
+      <c r="C6">
+        <v>0.9605263157894737</v>
+      </c>
+      <c r="D6">
+        <v>1.533333333333333</v>
+      </c>
+      <c r="E6">
+        <v>1.311111111111111</v>
+      </c>
+      <c r="F6">
+        <v>0.5051903114186851</v>
+      </c>
+      <c r="G6">
+        <v>0.7584541062801933</v>
+      </c>
+      <c r="H6">
+        <v>1.59958932238193</v>
+      </c>
+      <c r="I6">
+        <v>0.8294036061026352</v>
+      </c>
+      <c r="J6">
+        <v>1.139900662251656</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>GC_Mitotic</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>GC_Mural</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>3.314516129032258</v>
+      </c>
+      <c r="C8">
+        <v>2.793859649122807</v>
+      </c>
+      <c r="D8">
+        <v>3.607407407407408</v>
+      </c>
+      <c r="E8">
+        <v>1.897777777777778</v>
+      </c>
+      <c r="F8">
+        <v>1.916955017301038</v>
+      </c>
+      <c r="G8">
+        <v>2.449275362318841</v>
+      </c>
+      <c r="H8">
+        <v>3.151950718685832</v>
+      </c>
+      <c r="I8">
+        <v>2.06380027739251</v>
+      </c>
+      <c r="J8">
+        <v>2.502483443708609</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Granulosa</t>
+        </is>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Immune</t>
+        </is>
+      </c>
+      <c r="B10">
+        <v>0.1854838709677419</v>
+      </c>
+      <c r="C10">
+        <v>0.06140350877192982</v>
+      </c>
+      <c r="D10">
+        <v>0.08888888888888889</v>
+      </c>
+      <c r="E10">
+        <v>0.07555555555555556</v>
+      </c>
+      <c r="F10">
+        <v>0.04498269896193772</v>
+      </c>
+      <c r="G10">
+        <v>0.0821256038647343</v>
+      </c>
+      <c r="H10">
+        <v>0.1006160164271047</v>
+      </c>
+      <c r="I10">
+        <v>0.0651872399445215</v>
+      </c>
+      <c r="J10">
+        <v>0.07947019867549669</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>M_Early Theca</t>
+        </is>
+      </c>
+      <c r="B11">
+        <v>0.8145161290322581</v>
+      </c>
+      <c r="C11">
+        <v>0.5657894736842105</v>
+      </c>
+      <c r="D11">
+        <v>0.7555555555555555</v>
+      </c>
+      <c r="E11">
+        <v>0.4888888888888889</v>
+      </c>
+      <c r="F11">
+        <v>0.7093425605536332</v>
+      </c>
+      <c r="G11">
+        <v>0.4830917874396135</v>
+      </c>
+      <c r="H11">
+        <v>0.6817248459958932</v>
+      </c>
+      <c r="I11">
+        <v>0.5755894590846047</v>
+      </c>
+      <c r="J11">
+        <v>0.6183774834437086</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>M_Fibroblast-like Stroma</t>
+        </is>
+      </c>
+      <c r="B12">
+        <v>0.1209677419354839</v>
+      </c>
+      <c r="C12">
+        <v>0.03947368421052631</v>
+      </c>
+      <c r="D12">
+        <v>0.05185185185185185</v>
+      </c>
+      <c r="E12">
+        <v>0.05777777777777778</v>
+      </c>
+      <c r="F12">
+        <v>0.03114186851211072</v>
+      </c>
+      <c r="G12">
+        <v>0.02898550724637681</v>
+      </c>
+      <c r="H12">
+        <v>0.06365503080082136</v>
+      </c>
+      <c r="I12">
+        <v>0.03883495145631068</v>
+      </c>
+      <c r="J12">
+        <v>0.04884105960264901</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>M_Pericyte</t>
+        </is>
+      </c>
+      <c r="B13">
+        <v>0.2580645161290323</v>
+      </c>
+      <c r="C13">
+        <v>0.1271929824561404</v>
+      </c>
+      <c r="D13">
+        <v>0.3925925925925926</v>
+      </c>
+      <c r="E13">
+        <v>0.07111111111111111</v>
+      </c>
+      <c r="F13">
+        <v>0.09342560553633218</v>
+      </c>
+      <c r="G13">
+        <v>0.1352657004830918</v>
+      </c>
+      <c r="H13">
+        <v>0.2340862422997947</v>
+      </c>
+      <c r="I13">
+        <v>0.09847434119278779</v>
+      </c>
+      <c r="J13">
+        <v>0.1531456953642384</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>M_Smooth Muscle</t>
+        </is>
+      </c>
+      <c r="B14">
+        <v>0.1612903225806452</v>
+      </c>
+      <c r="C14">
+        <v>0.06140350877192982</v>
+      </c>
+      <c r="D14">
+        <v>0.1481481481481481</v>
+      </c>
+      <c r="E14">
+        <v>0.06222222222222222</v>
+      </c>
+      <c r="F14">
+        <v>0.06920415224913495</v>
+      </c>
+      <c r="G14">
+        <v>0.0821256038647343</v>
+      </c>
+      <c r="H14">
+        <v>0.1108829568788501</v>
+      </c>
+      <c r="I14">
+        <v>0.07073509015256588</v>
+      </c>
+      <c r="J14">
+        <v>0.0869205298013245</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>M_Steroidogenic Stroma</t>
+        </is>
+      </c>
+      <c r="B15">
+        <v>3.040322580645161</v>
+      </c>
+      <c r="C15">
+        <v>0.9429824561403509</v>
+      </c>
+      <c r="D15">
+        <v>2.214814814814815</v>
+      </c>
+      <c r="E15">
+        <v>1.026666666666667</v>
+      </c>
+      <c r="F15">
+        <v>1.103806228373702</v>
+      </c>
+      <c r="G15">
+        <v>1.014492753623188</v>
+      </c>
+      <c r="H15">
+        <v>1.829568788501027</v>
+      </c>
+      <c r="I15">
+        <v>1.054091539528433</v>
+      </c>
+      <c r="J15">
+        <v>1.366721854304636</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>M_Steroidogenic Theca</t>
+        </is>
+      </c>
+      <c r="B16">
+        <v>1.814516129032258</v>
+      </c>
+      <c r="C16">
+        <v>0.6754385964912281</v>
+      </c>
+      <c r="D16">
+        <v>1.422222222222222</v>
+      </c>
+      <c r="E16">
+        <v>1.013333333333333</v>
+      </c>
+      <c r="F16">
+        <v>0.7058823529411765</v>
+      </c>
+      <c r="G16">
+        <v>0.9130434782608695</v>
+      </c>
+      <c r="H16">
+        <v>1.172484599589322</v>
+      </c>
+      <c r="I16">
+        <v>0.8613037447988904</v>
+      </c>
+      <c r="J16">
+        <v>0.9867549668874173</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Mesenchyme</t>
+        </is>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B18">
+        <v>14.60483870967742</v>
+      </c>
+      <c r="C18">
+        <v>7.62280701754386</v>
+      </c>
+      <c r="D18">
+        <v>12.19259259259259</v>
+      </c>
+      <c r="E18">
+        <v>7.44</v>
+      </c>
+      <c r="F18">
+        <v>6.58477508650519</v>
+      </c>
+      <c r="G18">
+        <v>7.555555555555555</v>
+      </c>
+      <c r="H18">
+        <v>10.66735112936345</v>
+      </c>
+      <c r="I18">
+        <v>7.130374479889043</v>
+      </c>
+      <c r="J18">
+        <v>8.556291390728477</v>
       </c>
     </row>
   </sheetData>

</xml_diff>